<commit_message>
Script work continue TC - TMTT0033378 - 9th Aug 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
+++ b/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB611D6-D254-4FDE-A07C-F62FA7F77C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463BC50E-73E3-4833-A544-E20C0B93BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="ExternalContact" sheetId="12" r:id="rId2"/>
     <sheet name="Sections" sheetId="13" r:id="rId3"/>
     <sheet name="ContactInfoFields" sheetId="14" r:id="rId4"/>
+    <sheet name="TopRelationships" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Users</t>
   </si>
@@ -64,6 +65,21 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Contact Name:</t>
+  </si>
+  <si>
+    <t>Strength Rating:</t>
+  </si>
+  <si>
+    <t>Type:</t>
+  </si>
+  <si>
+    <t># Activities:</t>
+  </si>
+  <si>
+    <t>Last Activity Date:</t>
   </si>
 </sst>
 </file>
@@ -490,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30D0501-42CC-4BD6-8AC1-512324638DE3}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -517,4 +533,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539B3E85-C25E-4877-8532-7CF117E00909}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Script continue - TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage - 11 Aug 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
+++ b/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463BC50E-73E3-4833-A544-E20C0B93BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF75EEC-E234-4E8D-92A6-241484307169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sections" sheetId="13" r:id="rId3"/>
     <sheet name="ContactInfoFields" sheetId="14" r:id="rId4"/>
     <sheet name="TopRelationships" sheetId="15" r:id="rId5"/>
+    <sheet name="AffiliatedCompanies" sheetId="16" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Users</t>
   </si>
@@ -80,6 +81,12 @@
   </si>
   <si>
     <t>Last Activity Date:</t>
+  </si>
+  <si>
+    <t>Company Name:</t>
+  </si>
+  <si>
+    <t>Company Type:</t>
   </si>
 </sst>
 </file>
@@ -539,35 +546,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539B3E85-C25E-4877-8532-7CF117E00909}">
   <dimension ref="A1:A5"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F77889-4657-46E6-9E00-DF43D1296FD9}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final changes script - TMTT0033378 - 11 Aug 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
+++ b/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF75EEC-E234-4E8D-92A6-241484307169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01180601-BDB3-4556-9582-E4D6D113AAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ContactInfoFields" sheetId="14" r:id="rId4"/>
     <sheet name="TopRelationships" sheetId="15" r:id="rId5"/>
     <sheet name="AffiliatedCompanies" sheetId="16" r:id="rId6"/>
+    <sheet name="AssociatedEngagements" sheetId="17" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Users</t>
   </si>
@@ -87,6 +88,18 @@
   </si>
   <si>
     <t>Company Type:</t>
+  </si>
+  <si>
+    <t>Engagement:</t>
+  </si>
+  <si>
+    <t>Client Name:</t>
+  </si>
+  <si>
+    <t>Job Type:</t>
+  </si>
+  <si>
+    <t>Role:</t>
   </si>
 </sst>
 </file>
@@ -584,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F77889-4657-46E6-9E00-DF43D1296FD9}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -608,4 +621,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A608CA-96F0-4762-83F1-6AB77C030995}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Script work continue - 14 Aug 2023 TC - TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage
</commit_message>
<xml_diff>
--- a/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
+++ b/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01180601-BDB3-4556-9582-E4D6D113AAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A7EAFB-ABBD-427F-9ECB-03322F02581A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="ExternalContact" sheetId="12" r:id="rId2"/>
-    <sheet name="Sections" sheetId="13" r:id="rId3"/>
-    <sheet name="ContactInfoFields" sheetId="14" r:id="rId4"/>
-    <sheet name="TopRelationships" sheetId="15" r:id="rId5"/>
-    <sheet name="AffiliatedCompanies" sheetId="16" r:id="rId6"/>
-    <sheet name="AssociatedEngagements" sheetId="17" r:id="rId7"/>
+    <sheet name="EngContact" sheetId="18" r:id="rId3"/>
+    <sheet name="Sections" sheetId="13" r:id="rId4"/>
+    <sheet name="ContactInfoFields" sheetId="14" r:id="rId5"/>
+    <sheet name="TopRelationships" sheetId="15" r:id="rId6"/>
+    <sheet name="AffiliatedCompanies" sheetId="16" r:id="rId7"/>
+    <sheet name="AssociatedEngagements" sheetId="17" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Users</t>
   </si>
@@ -100,6 +101,12 @@
   </si>
   <si>
     <t>Role:</t>
+  </si>
+  <si>
+    <t>Aaron Rosen</t>
+  </si>
+  <si>
+    <t>Engagement Contact Name</t>
   </si>
 </sst>
 </file>
@@ -457,9 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4148951-CE41-4971-9C40-34811CD56C4D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -483,6 +488,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BF2CD7-0433-4F14-A411-F886B0A45EEF}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F224B8-81FE-41C4-8124-C11C3FDDBD17}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -522,7 +552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30D0501-42CC-4BD6-8AC1-512324638DE3}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -555,7 +585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539B3E85-C25E-4877-8532-7CF117E00909}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -593,7 +623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F77889-4657-46E6-9E00-DF43D1296FD9}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -623,11 +653,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A608CA-96F0-4762-83F1-6AB77C030995}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final changes - 23 Aug 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
+++ b/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A7EAFB-ABBD-427F-9ECB-03322F02581A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120B57B3-8CE2-4311-A69E-8A7BB42EFC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>Thomas Bailey</t>
   </si>
   <si>
-    <t>External Contact Name</t>
-  </si>
-  <si>
     <t>Aaron M. Rosen</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Engagement Contact Name</t>
+  </si>
+  <si>
+    <t>Ramana Sail</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4148951-CE41-4971-9C40-34811CD56C4D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -472,13 +474,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -491,20 +493,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BF2CD7-0433-4F14-A411-F886B0A45EEF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -524,27 +526,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -567,17 +569,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -595,27 +597,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -635,17 +637,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -665,22 +667,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1st Update - 28 Aug 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
+++ b/TestData/TMTT0033378_VerifyTheFunctionalityOfRelationshipTreemapAddedToExternalContactDetailPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120B57B3-8CE2-4311-A69E-8A7BB42EFC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAF1590-FF62-4875-8002-CA293320B9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="748" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="TopRelationships" sheetId="15" r:id="rId6"/>
     <sheet name="AffiliatedCompanies" sheetId="16" r:id="rId7"/>
     <sheet name="AssociatedEngagements" sheetId="17" r:id="rId8"/>
+    <sheet name="Referrals" sheetId="19" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Users</t>
   </si>
@@ -107,6 +108,15 @@
   </si>
   <si>
     <t>Ramana Sail</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Status:</t>
+  </si>
+  <si>
+    <t>Date Engaged:</t>
   </si>
 </sst>
 </file>
@@ -464,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4148951-CE41-4971-9C40-34811CD56C4D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -688,4 +698,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50F59D9-F042-4EC6-BA60-68464666625A}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>